<commit_message>
Updated reporting terminology from '実績' to '見込み'
</commit_message>
<xml_diff>
--- a/api/components/デイリーテンプレート.xlsx
+++ b/api/components/デイリーテンプレート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\almeida.ped_redhorse\Documents\GitHub\rht-hotel\api\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2133F8AD-D5DA-451C-B7B4-CABB83317296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A420762A-1B82-4CC3-8F04-56A5D8EDC740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-1670" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24210" yWindow="-1300" windowWidth="21600" windowHeight="18100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="レポート" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>月度</t>
   </si>
@@ -65,9 +65,6 @@
     <t>前日実績売上</t>
   </si>
   <si>
-    <t>前日実績稼働率</t>
-  </si>
-  <si>
     <t>前日確定泊数</t>
   </si>
   <si>
@@ -78,10 +75,6 @@
   </si>
   <si>
     <t>正味販売可能室数</t>
-  </si>
-  <si>
-    <t>実績稼働率</t>
-    <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>計画売上（百万円)</t>
@@ -121,9 +114,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>実績売上</t>
-  </si>
-  <si>
     <t>前年売上</t>
   </si>
   <si>
@@ -143,24 +133,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>実績売上（百万円)</t>
-    <rPh sb="5" eb="8">
-      <t>ヒャクマンエン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>計画売上（万円)</t>
-    <rPh sb="5" eb="6">
-      <t>マン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>エン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>実績売上（万円)</t>
     <rPh sb="5" eb="6">
       <t>マン</t>
     </rPh>
@@ -184,29 +157,45 @@
     <t>売上差異</t>
   </si>
   <si>
-    <t>実績稼働率</t>
-  </si>
-  <si>
     <t>稼働率差異</t>
-  </si>
-  <si>
-    <t>実績 ADR</t>
   </si>
   <si>
     <t>計画 ADR</t>
   </si>
   <si>
-    <t>実績 RevPAR</t>
-  </si>
-  <si>
     <t>計画 RevPAR</t>
   </si>
   <si>
-    <t>実績売上</t>
+    <t>確定泊数</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>確定泊数</t>
+    <t>売上</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>稼働率</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>前日稼働率</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>売上（百万円)</t>
+    <rPh sb="3" eb="6">
+      <t>ヒャクマンエン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>売上（万円)</t>
+    <rPh sb="3" eb="4">
+      <t>マン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>エン</t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -501,7 +490,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
-              <a:t>売上　計画ｘ実績</a:t>
+              <a:t>売上　計画ｘ見込み</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -677,7 +666,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 実績売上（百万円) </c:v>
+                  <c:v> 売上（百万円) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1237,7 +1226,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP" altLang="en-US" b="1"/>
-              <a:t>稼働率　計画ｘ実績</a:t>
+              <a:t>稼働率　計画ｘ見込み</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1404,7 +1393,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>実績稼働率</c:v>
+                  <c:v>稼働率</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1543,7 +1532,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>前日実績稼働率</c:v>
+                  <c:v>前日稼働率</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2204,7 +2193,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ja-JP"/>
-              <a:t>売上　計画ｘ実績</a:t>
+              <a:t>売上　計画ｘ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>見込み</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2379,7 +2372,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> 実績売上（万円) </c:v>
+                  <c:v> 売上（万円) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2827,7 +2820,11 @@
             </a:r>
             <a:r>
               <a:rPr lang="ja-JP"/>
-              <a:t>　計画ｘ実績</a:t>
+              <a:t>　計画ｘ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>見込み</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2999,7 +2996,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>実績稼働率</c:v>
+                  <c:v>稼働率</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5932,7 +5929,7 @@
   </sheetPr>
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -5941,7 +5938,7 @@
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="14" t="str">
         <f ca="1">_xlfn.CONCAT("デイリーレポート - ",TEXT(TODAY(),"yy年mm月dd日"))</f>
-        <v>デイリーレポート - 26年01月05日</v>
+        <v>デイリーレポート - 26年01月08日</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -5953,13 +5950,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
@@ -6171,7 +6168,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>2</v>
@@ -6180,7 +6177,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>4</v>
@@ -6189,37 +6186,37 @@
         <v>5</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.5">
@@ -6440,25 +6437,25 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H10" t="s">
         <v>3</v>
@@ -6467,25 +6464,25 @@
         <v>30</v>
       </c>
       <c r="J10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="L10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
@@ -6502,7 +6499,7 @@
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11" s="2" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="N11" s="11"/>
       <c r="O11" s="12">
@@ -6520,17 +6517,17 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="M12" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="M13" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="M14" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(report): split future months into separate Excel sheets and fix results aggregation
- Separated M+1 and M+2 data into '合計データ2' and '合計データ3' sheets.
- Set header row to 2 and data starting row to 3 for future months.
- Fixed NaN issues in total occupancy aggregation.
- Corrected hotel open date calculation for previous year metrics.
</commit_message>
<xml_diff>
--- a/api/components/デイリーテンプレート.xlsx
+++ b/api/components/デイリーテンプレート.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakamura.yos_redhors\Documents\GitHub\rht-hotel\api\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFB270-3E24-441A-9A89-ABD3A8205DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D6566-73F3-48D1-A301-E60BF8CFB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37980" yWindow="-3195" windowWidth="34455" windowHeight="14130" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37770" yWindow="-2745" windowWidth="18450" windowHeight="19470" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="レポート" sheetId="1" r:id="rId1"/>
@@ -301,9 +301,9 @@
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -401,6 +401,13 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans JP"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -483,7 +490,7 @@
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -516,11 +523,10 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -529,6 +535,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -740,6 +759,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.38045937938715307"/>
+          <c:y val="3.0530176344822715E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2582,63 +2609,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3430,63 +3401,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -4604,63 +4519,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -5452,63 +5311,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -6300,63 +6103,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -6896,63 +6643,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ja-JP" altLang="en-US"/>
-              <a:t>　　</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -12542,15 +12233,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>62865</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>59055</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>100965</xdr:rowOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>97154</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12580,15 +12271,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>64770</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>59689</xdr:rowOff>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>102869</xdr:rowOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>99058</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12656,15 +12347,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>161</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>208</xdr:row>
-      <xdr:rowOff>97155</xdr:rowOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>93344</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12694,15 +12385,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>267</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>314</xdr:row>
-      <xdr:rowOff>97155</xdr:rowOff>
+      <xdr:row>309</xdr:row>
+      <xdr:rowOff>93344</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12729,278 +12420,18 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>118828</xdr:colOff>
-          <xdr:row>55</xdr:row>
-          <xdr:rowOff>125730</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>669373</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>17145</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="図 8">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C31F6C-A9AA-1608-2CE0-BE5F6DD891DB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ!$A$9" spid="_x0000_s1135"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1738078" y="12336780"/>
-              <a:ext cx="3785235" cy="339090"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>115970</xdr:colOff>
-          <xdr:row>161</xdr:row>
-          <xdr:rowOff>64770</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>668420</xdr:colOff>
-          <xdr:row>162</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="11" name="図 10">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37B68EC2-D82A-93BE-1B3A-6525373D592A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ2!$A$1" spid="_x0000_s1136"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1735220" y="23886795"/>
-              <a:ext cx="3787140" cy="344805"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>112160</xdr:colOff>
-          <xdr:row>267</xdr:row>
-          <xdr:rowOff>93345</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>664610</xdr:colOff>
-          <xdr:row>268</xdr:row>
-          <xdr:rowOff>207645</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="12" name="図 11">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B578BC-0D56-0466-175B-A4F90AA1A790}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ3!$A$1" spid="_x0000_s1137"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1731410" y="35526345"/>
-              <a:ext cx="3794760" cy="337185"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>115970</xdr:colOff>
-          <xdr:row>107</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>666515</xdr:colOff>
-          <xdr:row>109</xdr:row>
-          <xdr:rowOff>95250</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="13" name="図 12">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F07EFE0-18EB-821D-DDC7-9D905BF679A0}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ!$H$9" spid="_x0000_s1138"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1735220" y="47015400"/>
-              <a:ext cx="3792855" cy="339090"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>59055</xdr:colOff>
-      <xdr:row>213</xdr:row>
-      <xdr:rowOff>88264</xdr:rowOff>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>212</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>261</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:row>257</xdr:row>
+      <xdr:rowOff>131444</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13021,89 +12452,24 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>114065</xdr:colOff>
-          <xdr:row>213</xdr:row>
-          <xdr:rowOff>167640</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>666515</xdr:colOff>
-          <xdr:row>215</xdr:row>
-          <xdr:rowOff>55245</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="18" name="図 17">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88B42E3F-A36B-BB01-F60E-8FDF86323933}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ2!$H$1" spid="_x0000_s1139"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1733315" y="58603515"/>
-              <a:ext cx="3794760" cy="329565"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>55245</xdr:colOff>
-      <xdr:row>319</xdr:row>
-      <xdr:rowOff>92074</xdr:rowOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>721525</xdr:colOff>
-      <xdr:row>367</xdr:row>
-      <xdr:rowOff>125729</xdr:rowOff>
+      <xdr:row>362</xdr:row>
+      <xdr:rowOff>131443</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13124,77 +12490,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>115018</xdr:colOff>
-          <xdr:row>319</xdr:row>
-          <xdr:rowOff>217170</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>669373</xdr:colOff>
-          <xdr:row>321</xdr:row>
-          <xdr:rowOff>116205</xdr:rowOff>
-        </xdr:to>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="21" name="図 20">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12068D11-8652-DEC9-D88E-3F0ACFD5B53A}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr>
-              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-              <a:extLst>
-                <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="合計データ3!$H$1" spid="_x0000_s1140"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPicPr>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-            <a:srcRect/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="1734268" y="70264020"/>
-              <a:ext cx="3792855" cy="337185"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:pic>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -13373,31 +12674,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I372"/>
+  <dimension ref="A1:I367"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="34" t="str">
+      <c r="A1" s="33" t="str">
         <f ca="1">_xlfn.CONCAT("デイリーレポート - ",TEXT(TODAY(),"yy年mm月dd日"))</f>
-        <v>デイリーレポート - 26年01月21日</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+        <v>デイリーレポート - 26年01月22日</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="17" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="18" ht="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -13548,296 +12852,338 @@
       <c r="H51" s="24"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A52" s="33"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A53" s="33"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A54" s="33"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
     </row>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="90" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="91" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="92" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="93" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="94" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="95" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="96" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="56" spans="1:9" ht="26.4" x14ac:dyDescent="0.65">
+      <c r="C56" s="39" t="str">
+        <f>合計データ!A9</f>
+        <v>売上　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A104" s="32">
+        <f>$A$52</f>
+        <v>0</v>
+      </c>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
+    </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A105" s="33">
-        <f>$A$52</f>
-        <v>0</v>
-      </c>
-      <c r="B105" s="33"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="33"/>
-      <c r="E105" s="33"/>
-      <c r="F105" s="33"/>
-      <c r="G105" s="33"/>
-      <c r="H105" s="33"/>
-      <c r="I105" s="33"/>
+      <c r="A105" s="32"/>
+      <c r="B105" s="32"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="32"/>
+      <c r="G105" s="32"/>
+      <c r="H105" s="32"/>
+      <c r="I105" s="32"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A106" s="33"/>
-      <c r="B106" s="33"/>
-      <c r="C106" s="33"/>
-      <c r="D106" s="33"/>
-      <c r="E106" s="33"/>
-      <c r="F106" s="33"/>
-      <c r="G106" s="33"/>
-      <c r="H106" s="33"/>
-      <c r="I106" s="33"/>
+      <c r="A106" s="32"/>
+      <c r="B106" s="32"/>
+      <c r="C106" s="32"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="32"/>
+      <c r="G106" s="32"/>
+      <c r="H106" s="32"/>
+      <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A107" s="33"/>
-      <c r="B107" s="33"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="33"/>
-      <c r="E107" s="33"/>
-      <c r="F107" s="33"/>
-      <c r="G107" s="33"/>
-      <c r="H107" s="33"/>
-      <c r="I107" s="33"/>
+    <row r="108" spans="1:9" ht="26.4" x14ac:dyDescent="0.65">
+      <c r="C108" s="39" t="str">
+        <f>合計データ!H9</f>
+        <v>稼働率　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D108" s="38"/>
+      <c r="E108" s="38"/>
+      <c r="F108" s="38"/>
+      <c r="G108" s="38"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A156" s="32">
+        <f>$A$52</f>
+        <v>0</v>
+      </c>
+      <c r="B156" s="32"/>
+      <c r="C156" s="32"/>
+      <c r="D156" s="32"/>
+      <c r="E156" s="32"/>
+      <c r="F156" s="32"/>
+      <c r="G156" s="32"/>
+      <c r="H156" s="32"/>
+      <c r="I156" s="32"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A157" s="32"/>
+      <c r="B157" s="32"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="32"/>
+      <c r="E157" s="32"/>
+      <c r="F157" s="32"/>
+      <c r="G157" s="32"/>
+      <c r="H157" s="32"/>
+      <c r="I157" s="32"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A158" s="33">
+      <c r="A158" s="32"/>
+      <c r="B158" s="32"/>
+      <c r="C158" s="32"/>
+      <c r="D158" s="32"/>
+      <c r="E158" s="32"/>
+      <c r="F158" s="32"/>
+      <c r="G158" s="32"/>
+      <c r="H158" s="32"/>
+      <c r="I158" s="32"/>
+    </row>
+    <row r="160" spans="1:9" ht="26.4" x14ac:dyDescent="0.65">
+      <c r="C160" s="39" t="str">
+        <f>合計データ2!A1</f>
+        <v>売上　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D160" s="39"/>
+      <c r="E160" s="39"/>
+      <c r="F160" s="39"/>
+      <c r="G160" s="39"/>
+    </row>
+    <row r="161" spans="3:7" s="37" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="C161" s="36"/>
+      <c r="D161" s="36"/>
+      <c r="E161" s="36"/>
+      <c r="F161" s="36"/>
+      <c r="G161" s="36"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A208" s="32">
         <f>$A$52</f>
         <v>0</v>
       </c>
-      <c r="B158" s="33"/>
-      <c r="C158" s="33"/>
-      <c r="D158" s="33"/>
-      <c r="E158" s="33"/>
-      <c r="F158" s="33"/>
-      <c r="G158" s="33"/>
-      <c r="H158" s="33"/>
-      <c r="I158" s="33"/>
+      <c r="B208" s="32"/>
+      <c r="C208" s="32"/>
+      <c r="D208" s="32"/>
+      <c r="E208" s="32"/>
+      <c r="F208" s="32"/>
+      <c r="G208" s="32"/>
+      <c r="H208" s="32"/>
+      <c r="I208" s="32"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A159" s="33"/>
-      <c r="B159" s="33"/>
-      <c r="C159" s="33"/>
-      <c r="D159" s="33"/>
-      <c r="E159" s="33"/>
-      <c r="F159" s="33"/>
-      <c r="G159" s="33"/>
-      <c r="H159" s="33"/>
-      <c r="I159" s="33"/>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A209" s="32"/>
+      <c r="B209" s="32"/>
+      <c r="C209" s="32"/>
+      <c r="D209" s="32"/>
+      <c r="E209" s="32"/>
+      <c r="F209" s="32"/>
+      <c r="G209" s="32"/>
+      <c r="H209" s="32"/>
+      <c r="I209" s="32"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A160" s="33"/>
-      <c r="B160" s="33"/>
-      <c r="C160" s="33"/>
-      <c r="D160" s="33"/>
-      <c r="E160" s="33"/>
-      <c r="F160" s="33"/>
-      <c r="G160" s="33"/>
-      <c r="H160" s="33"/>
-      <c r="I160" s="33"/>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A210" s="32"/>
+      <c r="B210" s="32"/>
+      <c r="C210" s="32"/>
+      <c r="D210" s="32"/>
+      <c r="E210" s="32"/>
+      <c r="F210" s="32"/>
+      <c r="G210" s="32"/>
+      <c r="H210" s="32"/>
+      <c r="I210" s="32"/>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A211" s="33">
+    <row r="212" spans="1:9" s="37" customFormat="1" ht="26.4" x14ac:dyDescent="0.65">
+      <c r="C212" s="40" t="str">
+        <f>合計データ2!H1</f>
+        <v>稼働率　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D212" s="39"/>
+      <c r="E212" s="39"/>
+      <c r="F212" s="39"/>
+      <c r="G212" s="39"/>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A260" s="32">
         <f>$A$52</f>
         <v>0</v>
       </c>
-      <c r="B211" s="33"/>
-      <c r="C211" s="33"/>
-      <c r="D211" s="33"/>
-      <c r="E211" s="33"/>
-      <c r="F211" s="33"/>
-      <c r="G211" s="33"/>
-      <c r="H211" s="33"/>
-      <c r="I211" s="33"/>
+      <c r="B260" s="32"/>
+      <c r="C260" s="32"/>
+      <c r="D260" s="32"/>
+      <c r="E260" s="32"/>
+      <c r="F260" s="32"/>
+      <c r="G260" s="32"/>
+      <c r="H260" s="32"/>
+      <c r="I260" s="32"/>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A212" s="33"/>
-      <c r="B212" s="33"/>
-      <c r="C212" s="33"/>
-      <c r="D212" s="33"/>
-      <c r="E212" s="33"/>
-      <c r="F212" s="33"/>
-      <c r="G212" s="33"/>
-      <c r="H212" s="33"/>
-      <c r="I212" s="33"/>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A261" s="32"/>
+      <c r="B261" s="32"/>
+      <c r="C261" s="32"/>
+      <c r="D261" s="32"/>
+      <c r="E261" s="32"/>
+      <c r="F261" s="32"/>
+      <c r="G261" s="32"/>
+      <c r="H261" s="32"/>
+      <c r="I261" s="32"/>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A213" s="33"/>
-      <c r="B213" s="33"/>
-      <c r="C213" s="33"/>
-      <c r="D213" s="33"/>
-      <c r="E213" s="33"/>
-      <c r="F213" s="33"/>
-      <c r="G213" s="33"/>
-      <c r="H213" s="33"/>
-      <c r="I213" s="33"/>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A262" s="32"/>
+      <c r="B262" s="32"/>
+      <c r="C262" s="32"/>
+      <c r="D262" s="32"/>
+      <c r="E262" s="32"/>
+      <c r="F262" s="32"/>
+      <c r="G262" s="32"/>
+      <c r="H262" s="32"/>
+      <c r="I262" s="32"/>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A264" s="33">
+    <row r="264" spans="1:9" ht="26.4" x14ac:dyDescent="0.65">
+      <c r="C264" s="39" t="str">
+        <f>合計データ3!A1</f>
+        <v>売上　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D264" s="38"/>
+      <c r="E264" s="38"/>
+      <c r="F264" s="38"/>
+      <c r="G264" s="38"/>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A312" s="32">
         <f>$A$52</f>
         <v>0</v>
       </c>
-      <c r="B264" s="33"/>
-      <c r="C264" s="33"/>
-      <c r="D264" s="33"/>
-      <c r="E264" s="33"/>
-      <c r="F264" s="33"/>
-      <c r="G264" s="33"/>
-      <c r="H264" s="33"/>
-      <c r="I264" s="33"/>
+      <c r="B312" s="32"/>
+      <c r="C312" s="32"/>
+      <c r="D312" s="32"/>
+      <c r="E312" s="32"/>
+      <c r="F312" s="32"/>
+      <c r="G312" s="32"/>
+      <c r="H312" s="32"/>
+      <c r="I312" s="32"/>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A265" s="33"/>
-      <c r="B265" s="33"/>
-      <c r="C265" s="33"/>
-      <c r="D265" s="33"/>
-      <c r="E265" s="33"/>
-      <c r="F265" s="33"/>
-      <c r="G265" s="33"/>
-      <c r="H265" s="33"/>
-      <c r="I265" s="33"/>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A313" s="32"/>
+      <c r="B313" s="32"/>
+      <c r="C313" s="32"/>
+      <c r="D313" s="32"/>
+      <c r="E313" s="32"/>
+      <c r="F313" s="32"/>
+      <c r="G313" s="32"/>
+      <c r="H313" s="32"/>
+      <c r="I313" s="32"/>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A266" s="33"/>
-      <c r="B266" s="33"/>
-      <c r="C266" s="33"/>
-      <c r="D266" s="33"/>
-      <c r="E266" s="33"/>
-      <c r="F266" s="33"/>
-      <c r="G266" s="33"/>
-      <c r="H266" s="33"/>
-      <c r="I266" s="33"/>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A314" s="32"/>
+      <c r="B314" s="32"/>
+      <c r="C314" s="32"/>
+      <c r="D314" s="32"/>
+      <c r="E314" s="32"/>
+      <c r="F314" s="32"/>
+      <c r="G314" s="32"/>
+      <c r="H314" s="32"/>
+      <c r="I314" s="32"/>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A317" s="33">
+    <row r="316" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="C316" s="40" t="str">
+        <f>合計データ3!H1</f>
+        <v>稼働率　計画ｘ見込み（1900年1月）</v>
+      </c>
+      <c r="D316" s="38"/>
+      <c r="E316" s="38"/>
+      <c r="F316" s="38"/>
+      <c r="G316" s="38"/>
+    </row>
+    <row r="317" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A365" s="32">
         <f>$A$52</f>
         <v>0</v>
       </c>
-      <c r="B317" s="33"/>
-      <c r="C317" s="33"/>
-      <c r="D317" s="33"/>
-      <c r="E317" s="33"/>
-      <c r="F317" s="33"/>
-      <c r="G317" s="33"/>
-      <c r="H317" s="33"/>
-      <c r="I317" s="33"/>
+      <c r="B365" s="32"/>
+      <c r="C365" s="32"/>
+      <c r="D365" s="32"/>
+      <c r="E365" s="32"/>
+      <c r="F365" s="32"/>
+      <c r="G365" s="32"/>
+      <c r="H365" s="32"/>
+      <c r="I365" s="32"/>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A318" s="33"/>
-      <c r="B318" s="33"/>
-      <c r="C318" s="33"/>
-      <c r="D318" s="33"/>
-      <c r="E318" s="33"/>
-      <c r="F318" s="33"/>
-      <c r="G318" s="33"/>
-      <c r="H318" s="33"/>
-      <c r="I318" s="33"/>
+    <row r="366" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A366" s="32"/>
+      <c r="B366" s="32"/>
+      <c r="C366" s="32"/>
+      <c r="D366" s="32"/>
+      <c r="E366" s="32"/>
+      <c r="F366" s="32"/>
+      <c r="G366" s="32"/>
+      <c r="H366" s="32"/>
+      <c r="I366" s="32"/>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A319" s="33"/>
-      <c r="B319" s="33"/>
-      <c r="C319" s="33"/>
-      <c r="D319" s="33"/>
-      <c r="E319" s="33"/>
-      <c r="F319" s="33"/>
-      <c r="G319" s="33"/>
-      <c r="H319" s="33"/>
-      <c r="I319" s="33"/>
-    </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A370" s="33">
-        <f>$A$52</f>
-        <v>0</v>
-      </c>
-      <c r="B370" s="33"/>
-      <c r="C370" s="33"/>
-      <c r="D370" s="33"/>
-      <c r="E370" s="33"/>
-      <c r="F370" s="33"/>
-      <c r="G370" s="33"/>
-      <c r="H370" s="33"/>
-      <c r="I370" s="33"/>
-    </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A371" s="33"/>
-      <c r="B371" s="33"/>
-      <c r="C371" s="33"/>
-      <c r="D371" s="33"/>
-      <c r="E371" s="33"/>
-      <c r="F371" s="33"/>
-      <c r="G371" s="33"/>
-      <c r="H371" s="33"/>
-      <c r="I371" s="33"/>
-    </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A372" s="33"/>
-      <c r="B372" s="33"/>
-      <c r="C372" s="33"/>
-      <c r="D372" s="33"/>
-      <c r="E372" s="33"/>
-      <c r="F372" s="33"/>
-      <c r="G372" s="33"/>
-      <c r="H372" s="33"/>
-      <c r="I372" s="33"/>
+    <row r="367" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A367" s="32"/>
+      <c r="B367" s="32"/>
+      <c r="C367" s="32"/>
+      <c r="D367" s="32"/>
+      <c r="E367" s="32"/>
+      <c r="F367" s="32"/>
+      <c r="G367" s="32"/>
+      <c r="H367" s="32"/>
+      <c r="I367" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A264:I266"/>
-    <mergeCell ref="A370:I372"/>
-    <mergeCell ref="A158:I160"/>
+  <mergeCells count="14">
+    <mergeCell ref="A260:I262"/>
+    <mergeCell ref="A365:I367"/>
+    <mergeCell ref="A156:I158"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A52:I54"/>
-    <mergeCell ref="A105:I107"/>
-    <mergeCell ref="A211:I213"/>
-    <mergeCell ref="A317:I319"/>
+    <mergeCell ref="A104:I106"/>
+    <mergeCell ref="A208:I210"/>
+    <mergeCell ref="A312:I314"/>
+    <mergeCell ref="C212:G212"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C160:G160"/>
+    <mergeCell ref="C264:G264"/>
+    <mergeCell ref="C316:G316"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C48:H48">
@@ -13857,17 +13203,20 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.28999999999999998" bottom="0.39370078740157483" header="0.63" footer="0.28999999999999998"/>
-  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;12&amp;KFFFFFFページ&amp;"Times New Roman,標準" &amp;P</oddFooter>
   </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
+  <rowBreaks count="6" manualBreakCount="6">
     <brk id="54" max="16383" man="1"/>
-    <brk id="107" max="16383" man="1"/>
+    <brk id="106" max="16383" man="1"/>
+    <brk id="158" max="16383" man="1"/>
+    <brk id="210" max="16383" man="1"/>
+    <brk id="262" max="16383" man="1"/>
+    <brk id="314" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -13878,8 +13227,8 @@
   </sheetPr>
   <dimension ref="A1:AE38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
@@ -13978,8 +13327,8 @@
       <c r="AB1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
     </row>
     <row r="2" spans="1:31" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="8"/>
@@ -14318,21 +13667,21 @@
       <c r="AB8" s="13"/>
     </row>
     <row r="9" spans="1:31" ht="26.4" x14ac:dyDescent="0.65">
-      <c r="A9" s="34" t="str">
+      <c r="A9" s="33" t="str">
         <f>"売上　計画ｘ見込み（" &amp; TEXT(B11, "yyyy年m月") &amp; "）"</f>
         <v>売上　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="34" t="str">
+      <c r="H9" s="33" t="str">
         <f>"稼働率　計画ｘ見込み（" &amp; TEXT(B11, "yyyy年m月") &amp; "）"</f>
         <v>稼働率　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
@@ -15148,7 +14497,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
@@ -15168,20 +14517,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="26.4" x14ac:dyDescent="0.65">
-      <c r="A1" s="34" t="str">
+      <c r="A1" s="33" t="str">
         <f>"売上　計画ｘ見込み（" &amp; TEXT(B3, "yyyy年m月") &amp; "）"</f>
         <v>売上　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="H1" s="36" t="str">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="H1" s="35" t="str">
         <f>"稼働率　計画ｘ見込み（" &amp; TEXT(B3, "yyyy年m月") &amp; "）"</f>
         <v>稼働率　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
@@ -15238,7 +14587,7 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="30"/>
+      <c r="I3" s="31"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
@@ -15264,7 +14613,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="13"/>
-      <c r="I4" s="30"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
       <c r="L4" s="14"/>
@@ -15290,7 +14639,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
-      <c r="I5" s="30"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
@@ -15316,7 +14665,7 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
-      <c r="I6" s="30"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -15342,7 +14691,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -15368,7 +14717,7 @@
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="I8" s="30"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -15394,7 +14743,7 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="13"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
@@ -15420,7 +14769,7 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -15446,7 +14795,7 @@
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -15472,7 +14821,7 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
-      <c r="I12" s="30"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -15498,7 +14847,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="13"/>
-      <c r="I13" s="30"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -15524,7 +14873,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
-      <c r="I14" s="30"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="14"/>
       <c r="K14" s="15"/>
       <c r="L14" s="14"/>
@@ -15550,7 +14899,7 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="14"/>
       <c r="K15" s="15"/>
       <c r="L15" s="14"/>
@@ -15576,7 +14925,7 @@
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="13"/>
-      <c r="I16" s="30"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
       <c r="L16" s="14"/>
@@ -15602,7 +14951,7 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="13"/>
-      <c r="I17" s="30"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
@@ -15628,7 +14977,7 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-      <c r="I18" s="30"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
       <c r="L18" s="14"/>
@@ -15654,7 +15003,7 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
-      <c r="I19" s="30"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
       <c r="L19" s="14"/>
@@ -15680,7 +15029,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
-      <c r="I20" s="30"/>
+      <c r="I20" s="31"/>
       <c r="J20" s="14"/>
       <c r="K20" s="15"/>
       <c r="L20" s="14"/>
@@ -15706,7 +15055,7 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="31"/>
       <c r="J21" s="14"/>
       <c r="K21" s="15"/>
       <c r="L21" s="14"/>
@@ -15732,7 +15081,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="14"/>
       <c r="K22" s="15"/>
       <c r="L22" s="14"/>
@@ -15758,7 +15107,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="14"/>
       <c r="K23" s="15"/>
       <c r="L23" s="14"/>
@@ -15784,7 +15133,7 @@
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="31"/>
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
       <c r="L24" s="14"/>
@@ -15810,7 +15159,7 @@
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
-      <c r="I25" s="30"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="14"/>
       <c r="K25" s="15"/>
       <c r="L25" s="14"/>
@@ -15836,7 +15185,7 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
-      <c r="I26" s="30"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="14"/>
       <c r="K26" s="15"/>
       <c r="L26" s="14"/>
@@ -15862,7 +15211,7 @@
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
-      <c r="I27" s="30"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="14"/>
       <c r="K27" s="15"/>
       <c r="L27" s="14"/>
@@ -15888,7 +15237,7 @@
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
-      <c r="I28" s="30"/>
+      <c r="I28" s="31"/>
       <c r="J28" s="14"/>
       <c r="K28" s="15"/>
       <c r="L28" s="14"/>
@@ -15914,7 +15263,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
-      <c r="I29" s="30"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="14"/>
       <c r="K29" s="15"/>
       <c r="L29" s="14"/>
@@ -15940,7 +15289,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
-      <c r="I30" s="30"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="14"/>
       <c r="K30" s="15"/>
       <c r="L30" s="14"/>
@@ -15983,7 +15332,7 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="L30" sqref="A3:L30"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
@@ -16003,20 +15352,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="26.4" x14ac:dyDescent="0.65">
-      <c r="A1" s="34" t="str">
+      <c r="A1" s="33" t="str">
         <f>"売上　計画ｘ見込み（" &amp; TEXT(B3, "yyyy年m月") &amp; "）"</f>
         <v>売上　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="H1" s="36" t="str">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="H1" s="35" t="str">
         <f>"稼働率　計画ｘ見込み（" &amp; TEXT(B3, "yyyy年m月") &amp; "）"</f>
         <v>稼働率　計画ｘ見込み（1900年1月）</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
@@ -16066,14 +15415,14 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3"/>
-      <c r="B3" s="30"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="30"/>
+      <c r="I3" s="31"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
@@ -16094,12 +15443,12 @@
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B4" s="30"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="11"/>
       <c r="F4" s="13"/>
-      <c r="I4" s="30"/>
+      <c r="I4" s="31"/>
       <c r="J4" s="14"/>
       <c r="K4" s="15"/>
       <c r="L4" s="14"/>
@@ -16120,12 +15469,12 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B5" s="30"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="11"/>
       <c r="F5" s="13"/>
-      <c r="I5" s="30"/>
+      <c r="I5" s="31"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
@@ -16146,12 +15495,12 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="11"/>
       <c r="F6" s="13"/>
-      <c r="I6" s="30"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -16172,12 +15521,12 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B7" s="30"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="11"/>
       <c r="F7" s="13"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -16198,12 +15547,12 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B8" s="30"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="11"/>
       <c r="F8" s="13"/>
-      <c r="I8" s="30"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -16224,12 +15573,12 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B9" s="30"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="11"/>
       <c r="F9" s="13"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
@@ -16250,12 +15599,12 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B10" s="30"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="11"/>
       <c r="F10" s="13"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="31"/>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -16276,12 +15625,12 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B11" s="30"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="11"/>
       <c r="F11" s="13"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="31"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -16302,12 +15651,12 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B12" s="30"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="11"/>
       <c r="F12" s="13"/>
-      <c r="I12" s="30"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -16328,12 +15677,12 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B13" s="30"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="11"/>
       <c r="F13" s="13"/>
-      <c r="I13" s="30"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -16354,12 +15703,12 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B14" s="30"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="11"/>
       <c r="F14" s="13"/>
-      <c r="I14" s="30"/>
+      <c r="I14" s="31"/>
       <c r="J14" s="14"/>
       <c r="K14" s="15"/>
       <c r="L14" s="14"/>
@@ -16380,12 +15729,12 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B15" s="30"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="11"/>
       <c r="F15" s="13"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="14"/>
       <c r="K15" s="15"/>
       <c r="L15" s="14"/>
@@ -16406,12 +15755,12 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="B16" s="30"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="11"/>
       <c r="F16" s="13"/>
-      <c r="I16" s="30"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
       <c r="L16" s="14"/>
@@ -16432,12 +15781,12 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B17" s="30"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="11"/>
       <c r="F17" s="13"/>
-      <c r="I17" s="30"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
@@ -16458,12 +15807,12 @@
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B18" s="30"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="11"/>
       <c r="F18" s="13"/>
-      <c r="I18" s="30"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
       <c r="L18" s="14"/>
@@ -16484,12 +15833,12 @@
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B19" s="30"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
       <c r="F19" s="13"/>
-      <c r="I19" s="30"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
       <c r="L19" s="14"/>
@@ -16510,12 +15859,12 @@
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B20" s="30"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="11"/>
       <c r="F20" s="13"/>
-      <c r="I20" s="30"/>
+      <c r="I20" s="31"/>
       <c r="J20" s="14"/>
       <c r="K20" s="15"/>
       <c r="L20" s="14"/>
@@ -16536,12 +15885,12 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B21" s="30"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="11"/>
       <c r="F21" s="13"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="31"/>
       <c r="J21" s="14"/>
       <c r="K21" s="15"/>
       <c r="L21" s="14"/>
@@ -16562,12 +15911,12 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B22" s="30"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="11"/>
       <c r="F22" s="13"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="14"/>
       <c r="K22" s="15"/>
       <c r="L22" s="14"/>
@@ -16588,12 +15937,12 @@
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B23" s="30"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="11"/>
       <c r="F23" s="13"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="14"/>
       <c r="K23" s="15"/>
       <c r="L23" s="14"/>
@@ -16614,12 +15963,12 @@
       <c r="R23" s="1"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B24" s="30"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="11"/>
       <c r="F24" s="13"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="31"/>
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
       <c r="L24" s="14"/>
@@ -16640,12 +15989,12 @@
       <c r="R24" s="1"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B25" s="30"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="11"/>
       <c r="F25" s="13"/>
-      <c r="I25" s="30"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="14"/>
       <c r="K25" s="15"/>
       <c r="L25" s="14"/>
@@ -16666,12 +16015,12 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B26" s="30"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="11"/>
       <c r="F26" s="13"/>
-      <c r="I26" s="30"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="14"/>
       <c r="K26" s="15"/>
       <c r="L26" s="14"/>
@@ -16692,12 +16041,12 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B27" s="30"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="11"/>
       <c r="F27" s="13"/>
-      <c r="I27" s="30"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="14"/>
       <c r="K27" s="15"/>
       <c r="L27" s="14"/>
@@ -16718,12 +16067,12 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B28" s="30"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="11"/>
       <c r="F28" s="13"/>
-      <c r="I28" s="30"/>
+      <c r="I28" s="31"/>
       <c r="J28" s="14"/>
       <c r="K28" s="15"/>
       <c r="L28" s="14"/>
@@ -16744,12 +16093,12 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B29" s="30"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="11"/>
       <c r="F29" s="13"/>
-      <c r="I29" s="30"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="14"/>
       <c r="K29" s="15"/>
       <c r="L29" s="14"/>
@@ -16770,12 +16119,12 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B30" s="30"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="11"/>
       <c r="F30" s="13"/>
-      <c r="I30" s="30"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="14"/>
       <c r="K30" s="15"/>
       <c r="L30" s="14"/>

</xml_diff>

<commit_message>
fix: Fixed the issue where the first row was hidden in the February/March sales graph.
</commit_message>
<xml_diff>
--- a/api/components/デイリーテンプレート.xlsx
+++ b/api/components/デイリーテンプレート.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakamura.yos_redhors\Documents\GitHub\rht-hotel\api\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakamura.yos_redhors\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F57DA32-F4C1-4CE9-86CB-CF86333D35F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{425D826B-7E67-4CC8-BB33-85A98290820E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35175" yWindow="-2430" windowWidth="31860" windowHeight="19695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37965" yWindow="-2640" windowWidth="30210" windowHeight="18930" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="レポート" sheetId="1" r:id="rId1"/>
@@ -1041,7 +1041,37 @@
     <cellStyle name="桁区切り 2" xfId="3" xr:uid="{FADD5BB4-22B4-4CE0-8B7D-319EB05B36C7}"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -4697,6 +4727,12 @@
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4811,88 +4847,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5008,88 +5050,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5203,88 +5251,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5705,6 +5759,12 @@
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5819,88 +5879,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6016,88 +6082,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6211,88 +6283,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8030,6 +8108,12 @@
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8144,88 +8228,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8341,88 +8431,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8536,88 +8632,94 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15210,7 +15312,7 @@
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="91" t="str">
         <f ca="1">_xlfn.CONCAT("デイリーレポート - ",TEXT(TODAY(),"yy年mm月dd日"))</f>
-        <v>デイリーレポート - 26年01月27日</v>
+        <v>デイリーレポート - 26年01月28日</v>
       </c>
       <c r="B1" s="91"/>
       <c r="C1" s="91"/>
@@ -15705,18 +15807,18 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="C48:H48">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:H51">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15745,9 +15847,7 @@
   </sheetPr>
   <dimension ref="A1:AE41"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
   <cols>
@@ -16274,17 +16374,17 @@
       <c r="L11" s="61"/>
       <c r="M11" s="70"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="10">
-        <f>C11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <f>D11/10000</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="10">
-        <f>E11/10000</f>
-        <v>0</v>
+      <c r="O11" s="10" t="e">
+        <f>IF($A11="",NA(),$C11/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" s="10" t="e">
+        <f>IF($A11="",NA(),$D11/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" s="10" t="e">
+        <f>IF($A11="",NA(),$E11/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R11" s="10" t="str">
         <f>IF(OR(F11="",F11=0),"",(D11+F11)/10000)</f>
@@ -16305,17 +16405,17 @@
       <c r="L12" s="33"/>
       <c r="M12" s="71"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="10">
-        <f t="shared" ref="O12:O38" si="6">C12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" ref="P12:P38" si="7">D12/10000</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="10">
-        <f t="shared" ref="Q12:Q38" si="8">E12/10000</f>
-        <v>0</v>
+      <c r="O12" s="10" t="e">
+        <f t="shared" ref="O12:O40" si="6">IF($A12="",NA(),$C12/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P12" s="10" t="e">
+        <f t="shared" ref="P12:P40" si="7">IF($A12="",NA(),$D12/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q12" s="10" t="e">
+        <f t="shared" ref="Q12:Q40" si="8">IF($A12="",NA(),$E12/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R12" s="10" t="str">
         <f t="shared" ref="R12:R38" si="9">IF(OR(F12="",F12=0),"",(D12+F12)/10000)</f>
@@ -16337,17 +16437,17 @@
       <c r="L13" s="61"/>
       <c r="M13" s="58"/>
       <c r="N13" s="7"/>
-      <c r="O13" s="10">
+      <c r="O13" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q13" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R13" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16368,17 +16468,17 @@
       <c r="L14" s="33"/>
       <c r="M14" s="71"/>
       <c r="N14" s="7"/>
-      <c r="O14" s="10">
+      <c r="O14" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P14" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R14" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16400,17 +16500,17 @@
       <c r="L15" s="61"/>
       <c r="M15" s="70"/>
       <c r="N15"/>
-      <c r="O15" s="10">
+      <c r="O15" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R15" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16431,17 +16531,17 @@
       <c r="L16" s="33"/>
       <c r="M16" s="71"/>
       <c r="N16"/>
-      <c r="O16" s="10">
+      <c r="O16" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P16" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R16" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16463,17 +16563,17 @@
       <c r="L17" s="61"/>
       <c r="M17" s="70"/>
       <c r="N17"/>
-      <c r="O17" s="10">
+      <c r="O17" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R17" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16494,17 +16594,17 @@
       <c r="L18" s="33"/>
       <c r="M18" s="71"/>
       <c r="N18"/>
-      <c r="O18" s="10">
+      <c r="O18" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P18" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R18" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16526,17 +16626,17 @@
       <c r="L19" s="61"/>
       <c r="M19" s="70"/>
       <c r="N19"/>
-      <c r="O19" s="10">
+      <c r="O19" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P19" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q19" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R19" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16557,17 +16657,17 @@
       <c r="L20" s="33"/>
       <c r="M20" s="71"/>
       <c r="N20"/>
-      <c r="O20" s="10">
+      <c r="O20" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R20" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16589,17 +16689,17 @@
       <c r="L21" s="61"/>
       <c r="M21" s="70"/>
       <c r="N21"/>
-      <c r="O21" s="10">
+      <c r="O21" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P21" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q21" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R21" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16620,17 +16720,17 @@
       <c r="L22" s="33"/>
       <c r="M22" s="71"/>
       <c r="N22"/>
-      <c r="O22" s="10">
+      <c r="O22" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P22" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q22" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R22" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16652,17 +16752,17 @@
       <c r="L23" s="61"/>
       <c r="M23" s="70"/>
       <c r="N23"/>
-      <c r="O23" s="10">
+      <c r="O23" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P23" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q23" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R23" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16683,17 +16783,17 @@
       <c r="L24" s="33"/>
       <c r="M24" s="71"/>
       <c r="N24"/>
-      <c r="O24" s="10">
+      <c r="O24" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P24" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q24" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R24" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16715,17 +16815,17 @@
       <c r="L25" s="61"/>
       <c r="M25" s="70"/>
       <c r="N25"/>
-      <c r="O25" s="10">
+      <c r="O25" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P25" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q25" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R25" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16746,17 +16846,17 @@
       <c r="L26" s="33"/>
       <c r="M26" s="71"/>
       <c r="N26"/>
-      <c r="O26" s="10">
+      <c r="O26" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P26" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q26" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R26" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16778,17 +16878,17 @@
       <c r="L27" s="61"/>
       <c r="M27" s="70"/>
       <c r="N27"/>
-      <c r="O27" s="10">
+      <c r="O27" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P27" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q27" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R27" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16809,17 +16909,17 @@
       <c r="L28" s="33"/>
       <c r="M28" s="43"/>
       <c r="N28"/>
-      <c r="O28" s="10">
+      <c r="O28" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P28" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q28" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R28" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16841,17 +16941,17 @@
       <c r="L29" s="61"/>
       <c r="M29" s="70"/>
       <c r="N29"/>
-      <c r="O29" s="10">
+      <c r="O29" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P29" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q29" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R29" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16872,17 +16972,17 @@
       <c r="L30" s="33"/>
       <c r="M30" s="71"/>
       <c r="N30"/>
-      <c r="O30" s="10">
+      <c r="O30" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P30" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q30" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R30" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16904,17 +17004,17 @@
       <c r="L31" s="61"/>
       <c r="M31" s="70"/>
       <c r="N31"/>
-      <c r="O31" s="10">
+      <c r="O31" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P31" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q31" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R31" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16935,17 +17035,17 @@
       <c r="L32" s="33"/>
       <c r="M32" s="71"/>
       <c r="N32"/>
-      <c r="O32" s="10">
+      <c r="O32" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P32" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q32" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R32" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16967,17 +17067,17 @@
       <c r="L33" s="61"/>
       <c r="M33" s="70"/>
       <c r="N33"/>
-      <c r="O33" s="10">
+      <c r="O33" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P33" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P33" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q33" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R33" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16998,17 +17098,17 @@
       <c r="L34" s="33"/>
       <c r="M34" s="71"/>
       <c r="N34"/>
-      <c r="O34" s="10">
+      <c r="O34" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P34" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P34" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q34" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R34" s="10" t="str">
         <f t="shared" si="9"/>
@@ -17030,17 +17130,17 @@
       <c r="L35" s="61"/>
       <c r="M35" s="70"/>
       <c r="N35"/>
-      <c r="O35" s="10">
+      <c r="O35" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P35" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q35" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q35" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R35" s="10" t="str">
         <f t="shared" si="9"/>
@@ -17061,17 +17161,17 @@
       <c r="L36" s="33"/>
       <c r="M36" s="71"/>
       <c r="N36"/>
-      <c r="O36" s="10">
+      <c r="O36" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P36" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q36" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q36" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R36" s="10" t="str">
         <f t="shared" si="9"/>
@@ -17093,17 +17193,17 @@
       <c r="L37" s="61"/>
       <c r="M37" s="70"/>
       <c r="N37"/>
-      <c r="O37" s="10">
+      <c r="O37" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P37" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q37" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q37" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R37" s="10" t="str">
         <f t="shared" si="9"/>
@@ -17124,17 +17224,17 @@
       <c r="L38" s="33"/>
       <c r="M38" s="71"/>
       <c r="N38"/>
-      <c r="O38" s="10">
+      <c r="O38" s="10" t="e">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="P38" s="10" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q38" s="10">
+        <v>#N/A</v>
+      </c>
+      <c r="Q38" s="10" t="e">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="R38" s="10" t="str">
         <f t="shared" si="9"/>
@@ -17155,6 +17255,22 @@
       <c r="K39" s="57"/>
       <c r="L39" s="61"/>
       <c r="M39" s="70"/>
+      <c r="O39" s="10" t="e">
+        <f t="shared" si="6"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P39" s="10" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q39" s="10" t="e">
+        <f t="shared" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R39" s="10" t="str">
+        <f t="shared" ref="R39:R40" si="10">IF(OR(F39="",F39=0),"",(D39+F39)/10000)</f>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A40" s="31"/>
@@ -17170,6 +17286,22 @@
       <c r="K40" s="73"/>
       <c r="L40" s="71"/>
       <c r="M40" s="71"/>
+      <c r="O40" s="10" t="e">
+        <f t="shared" si="6"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P40" s="10" t="e">
+        <f t="shared" si="7"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q40" s="10" t="e">
+        <f t="shared" si="8"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R40" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
@@ -17182,30 +17314,40 @@
     <mergeCell ref="H9:K9"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="E11:E40">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>$E11&lt;0</formula>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>$E40&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L11:L40">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>$L11&lt;0</formula>
+  <conditionalFormatting sqref="L40">
+    <cfRule type="expression" dxfId="14" priority="4">
+      <formula>$L40&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:AB3">
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W5:AB5">
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="21" operator="greaterThan">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E39">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$E11&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L39">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>$L11&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -17331,17 +17473,17 @@
       <c r="L3" s="61"/>
       <c r="M3" s="70"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="10">
-        <f>C3/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
-        <f>D3/10000</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="10">
-        <f>E3/10000</f>
-        <v>0</v>
+      <c r="O3" s="10" t="e">
+        <f>IF($A3="",NA(),$C3/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P3" s="10" t="e">
+        <f>IF($A3="",NA(),$D3/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q3" s="10" t="e">
+        <f>IF($A3="",NA(),$E3/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R3" s="10" t="str">
         <f>IF(OR(F3="",F3=0),"",(D3+F3)/10000)</f>
@@ -17363,20 +17505,20 @@
       <c r="L4" s="33"/>
       <c r="M4" s="71"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="10">
-        <f t="shared" ref="O4:O30" si="0">C4/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" ref="P4:P30" si="1">D4/10000</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="10">
-        <f t="shared" ref="Q4:Q30" si="2">E4/10000</f>
-        <v>0</v>
+      <c r="O4" s="10" t="e">
+        <f>IF($A4="",NA(),$C4/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P4" s="10" t="e">
+        <f>IF($A4="",NA(),$D4/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q4" s="10" t="e">
+        <f>IF($A4="",NA(),$E4/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R4" s="10" t="str">
-        <f t="shared" ref="R4:R30" si="3">IF(OR(F4="",F4=0),"",(D4+F4)/10000)</f>
+        <f t="shared" ref="R4:R30" si="0">IF(OR(F4="",F4=0),"",(D4+F4)/10000)</f>
         <v/>
       </c>
       <c r="S4" s="1"/>
@@ -17396,17 +17538,17 @@
       <c r="L5" s="61"/>
       <c r="M5" s="70"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="O5" s="10" t="e">
+        <f>IF($A5="",NA(),$C5/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P5" s="10" t="e">
+        <f>IF($A5="",NA(),$D5/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" s="10" t="e">
+        <f>IF($A5="",NA(),$E5/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R5" s="10" t="str">
         <f>IF(OR(F5="",F5=0),"",(D5+F5)/10000)</f>
@@ -17428,20 +17570,20 @@
       <c r="L6" s="33"/>
       <c r="M6" s="71"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="10">
+      <c r="O6" s="10" t="e">
+        <f t="shared" ref="O6:O32" si="1">IF($A6="",NA(),$C6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P6" s="10" t="e">
+        <f t="shared" ref="P6:P32" si="2">IF($A6="",NA(),$D6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" s="10" t="e">
+        <f t="shared" ref="Q6:Q32" si="3">IF($A6="",NA(),$E6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S6" s="1"/>
@@ -17461,20 +17603,20 @@
       <c r="L7" s="61"/>
       <c r="M7" s="70"/>
       <c r="N7"/>
-      <c r="O7" s="10">
+      <c r="O7" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P7" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q7" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S7" s="1"/>
@@ -17493,20 +17635,20 @@
       <c r="L8" s="33"/>
       <c r="M8" s="71"/>
       <c r="N8"/>
-      <c r="O8" s="10">
+      <c r="O8" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P8" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S8" s="1"/>
@@ -17526,20 +17668,20 @@
       <c r="L9" s="61"/>
       <c r="M9" s="58"/>
       <c r="N9"/>
-      <c r="O9" s="10">
+      <c r="O9" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S9" s="1"/>
@@ -17558,20 +17700,20 @@
       <c r="L10" s="33"/>
       <c r="M10" s="43"/>
       <c r="N10"/>
-      <c r="O10" s="10">
+      <c r="O10" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P10" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q10" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S10" s="1"/>
@@ -17591,20 +17733,20 @@
       <c r="L11" s="61"/>
       <c r="M11" s="70"/>
       <c r="N11"/>
-      <c r="O11" s="10">
+      <c r="O11" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S11" s="1"/>
@@ -17623,20 +17765,20 @@
       <c r="L12" s="33"/>
       <c r="M12" s="71"/>
       <c r="N12"/>
-      <c r="O12" s="10">
+      <c r="O12" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P12" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q12" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S12" s="1"/>
@@ -17656,20 +17798,20 @@
       <c r="L13" s="61"/>
       <c r="M13" s="58"/>
       <c r="N13"/>
-      <c r="O13" s="10">
+      <c r="O13" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q13" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S13" s="1"/>
@@ -17688,20 +17830,20 @@
       <c r="L14" s="33"/>
       <c r="M14" s="71"/>
       <c r="N14"/>
-      <c r="O14" s="10">
+      <c r="O14" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P14" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S14" s="1"/>
@@ -17721,20 +17863,20 @@
       <c r="L15" s="61"/>
       <c r="M15" s="70"/>
       <c r="N15"/>
-      <c r="O15" s="10">
+      <c r="O15" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S15" s="1"/>
@@ -17753,20 +17895,20 @@
       <c r="L16" s="33"/>
       <c r="M16" s="43"/>
       <c r="N16"/>
-      <c r="O16" s="10">
+      <c r="O16" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P16" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S16" s="1"/>
@@ -17786,20 +17928,20 @@
       <c r="L17" s="61"/>
       <c r="M17" s="70"/>
       <c r="N17"/>
-      <c r="O17" s="10">
+      <c r="O17" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S17" s="1"/>
@@ -17818,20 +17960,20 @@
       <c r="L18" s="33"/>
       <c r="M18" s="71"/>
       <c r="N18"/>
-      <c r="O18" s="10">
+      <c r="O18" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P18" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S18" s="1"/>
@@ -17851,20 +17993,20 @@
       <c r="L19" s="61"/>
       <c r="M19" s="70"/>
       <c r="N19"/>
-      <c r="O19" s="10">
+      <c r="O19" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P19" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q19" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R19" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S19" s="1"/>
@@ -17883,20 +18025,20 @@
       <c r="L20" s="33"/>
       <c r="M20" s="71"/>
       <c r="N20"/>
-      <c r="O20" s="10">
+      <c r="O20" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S20" s="1"/>
@@ -17916,20 +18058,20 @@
       <c r="L21" s="61"/>
       <c r="M21" s="70"/>
       <c r="N21"/>
-      <c r="O21" s="10">
+      <c r="O21" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P21" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q21" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R21" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S21" s="1"/>
@@ -17948,20 +18090,20 @@
       <c r="L22" s="33"/>
       <c r="M22" s="71"/>
       <c r="N22"/>
-      <c r="O22" s="10">
+      <c r="O22" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P22" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q22" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R22" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S22" s="1"/>
@@ -17981,20 +18123,20 @@
       <c r="L23" s="61"/>
       <c r="M23" s="70"/>
       <c r="N23"/>
-      <c r="O23" s="10">
+      <c r="O23" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P23" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q23" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R23" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S23" s="1"/>
@@ -18013,20 +18155,20 @@
       <c r="L24" s="33"/>
       <c r="M24" s="71"/>
       <c r="N24"/>
-      <c r="O24" s="10">
+      <c r="O24" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P24" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q24" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R24" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S24" s="1"/>
@@ -18046,20 +18188,20 @@
       <c r="L25" s="61"/>
       <c r="M25" s="70"/>
       <c r="N25"/>
-      <c r="O25" s="10">
+      <c r="O25" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P25" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q25" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R25" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S25" s="1"/>
@@ -18078,20 +18220,20 @@
       <c r="L26" s="33"/>
       <c r="M26" s="71"/>
       <c r="N26"/>
-      <c r="O26" s="10">
+      <c r="O26" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P26" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q26" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R26" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S26" s="1"/>
@@ -18111,20 +18253,20 @@
       <c r="L27" s="61"/>
       <c r="M27" s="70"/>
       <c r="N27"/>
-      <c r="O27" s="10">
+      <c r="O27" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P27" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q27" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R27" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S27" s="1"/>
@@ -18143,20 +18285,20 @@
       <c r="L28" s="33"/>
       <c r="M28" s="43"/>
       <c r="N28"/>
-      <c r="O28" s="10">
+      <c r="O28" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P28" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q28" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R28" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S28" s="1"/>
@@ -18176,20 +18318,20 @@
       <c r="L29" s="61"/>
       <c r="M29" s="70"/>
       <c r="N29"/>
-      <c r="O29" s="10">
+      <c r="O29" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P29" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q29" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R29" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S29" s="1"/>
@@ -18208,20 +18350,20 @@
       <c r="L30" s="33"/>
       <c r="M30" s="43"/>
       <c r="N30"/>
-      <c r="O30" s="10">
+      <c r="O30" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P30" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q30" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R30" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="10" t="str">
-        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="S30" s="1"/>
@@ -18240,6 +18382,22 @@
       <c r="K31" s="57"/>
       <c r="L31" s="61"/>
       <c r="M31" s="70"/>
+      <c r="O31" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P31" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q31" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R31" s="10" t="str">
+        <f t="shared" ref="R31:R32" si="4">IF(OR(F31="",F31=0),"",(D31+F31)/10000)</f>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" s="31"/>
@@ -18255,6 +18413,22 @@
       <c r="K32" s="73"/>
       <c r="L32" s="71"/>
       <c r="M32" s="71"/>
+      <c r="O32" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P32" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q32" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
@@ -18268,12 +18442,22 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="E3:E32">
+  <conditionalFormatting sqref="E32">
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>$E32&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>$L32&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E31">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$E3&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L32">
+  <conditionalFormatting sqref="L3:L31">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$L3&lt;0</formula>
     </cfRule>
@@ -18401,17 +18585,17 @@
       <c r="L3" s="61"/>
       <c r="M3" s="70"/>
       <c r="N3" s="8"/>
-      <c r="O3" s="10">
-        <f>C3/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
-        <f>D3/10000</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="10">
-        <f>E3/10000</f>
-        <v>0</v>
+      <c r="O3" s="10" t="e">
+        <f>IF($A3="",NA(),$C3/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P3" s="10" t="e">
+        <f>IF($A3="",NA(),$D3/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q3" s="10" t="e">
+        <f>IF($A3="",NA(),$E3/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R3" s="10" t="str">
         <f>IF(OR(F3="",F3=0),"",(D3+F3)/10000)</f>
@@ -18433,20 +18617,20 @@
       <c r="L4" s="33"/>
       <c r="M4" s="71"/>
       <c r="N4" s="7"/>
-      <c r="O4" s="10">
-        <f t="shared" ref="O4:Q30" si="0">C4/10000</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="O4" s="10" t="e">
+        <f>IF($A4="",NA(),$C4/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P4" s="10" t="e">
+        <f>IF($A4="",NA(),$D4/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q4" s="10" t="e">
+        <f>IF($A4="",NA(),$E4/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R4" s="10" t="str">
-        <f t="shared" ref="R4:R30" si="1">IF(OR(F4="",F4=0),"",(D4+F4)/10000)</f>
+        <f t="shared" ref="R4:R30" si="0">IF(OR(F4="",F4=0),"",(D4+F4)/10000)</f>
         <v/>
       </c>
       <c r="S4" s="1"/>
@@ -18466,17 +18650,17 @@
       <c r="L5" s="61"/>
       <c r="M5" s="58"/>
       <c r="N5" s="7"/>
-      <c r="O5" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="O5" s="10" t="e">
+        <f>IF($A5="",NA(),$C5/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P5" s="10" t="e">
+        <f>IF($A5="",NA(),$D5/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" s="10" t="e">
+        <f>IF($A5="",NA(),$E5/10000)</f>
+        <v>#N/A</v>
       </c>
       <c r="R5" s="10" t="str">
         <f>IF(OR(F5="",F5=0),"",(D5+F5)/10000)</f>
@@ -18498,20 +18682,20 @@
       <c r="L6" s="33"/>
       <c r="M6" s="43"/>
       <c r="N6" s="7"/>
-      <c r="O6" s="10">
+      <c r="O6" s="10" t="e">
+        <f t="shared" ref="O6:O32" si="1">IF($A6="",NA(),$C6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="P6" s="10" t="e">
+        <f t="shared" ref="P6:P32" si="2">IF($A6="",NA(),$D6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" s="10" t="e">
+        <f t="shared" ref="Q6:Q32" si="3">IF($A6="",NA(),$E6/10000)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R6" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S6" s="1"/>
@@ -18531,20 +18715,20 @@
       <c r="L7" s="61"/>
       <c r="M7" s="58"/>
       <c r="N7"/>
-      <c r="O7" s="10">
+      <c r="O7" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P7" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q7" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S7" s="1"/>
@@ -18563,20 +18747,20 @@
       <c r="L8" s="33"/>
       <c r="M8" s="71"/>
       <c r="N8"/>
-      <c r="O8" s="10">
+      <c r="O8" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P8" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P8" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S8" s="1"/>
@@ -18596,20 +18780,20 @@
       <c r="L9" s="61"/>
       <c r="M9" s="70"/>
       <c r="N9"/>
-      <c r="O9" s="10">
+      <c r="O9" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S9" s="1"/>
@@ -18626,22 +18810,22 @@
       <c r="J10" s="32"/>
       <c r="K10" s="37"/>
       <c r="L10" s="33"/>
-      <c r="M10" s="71"/>
+      <c r="M10" s="43"/>
       <c r="N10"/>
-      <c r="O10" s="10">
+      <c r="O10" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P10" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q10" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R10" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S10" s="1"/>
@@ -18661,20 +18845,20 @@
       <c r="L11" s="61"/>
       <c r="M11" s="70"/>
       <c r="N11"/>
-      <c r="O11" s="10">
+      <c r="O11" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S11" s="1"/>
@@ -18693,20 +18877,20 @@
       <c r="L12" s="33"/>
       <c r="M12" s="43"/>
       <c r="N12"/>
-      <c r="O12" s="10">
+      <c r="O12" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P12" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q12" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R12" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S12" s="1"/>
@@ -18726,20 +18910,20 @@
       <c r="L13" s="61"/>
       <c r="M13" s="70"/>
       <c r="N13"/>
-      <c r="O13" s="10">
+      <c r="O13" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q13" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S13" s="1"/>
@@ -18758,20 +18942,20 @@
       <c r="L14" s="33"/>
       <c r="M14" s="71"/>
       <c r="N14"/>
-      <c r="O14" s="10">
+      <c r="O14" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P14" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S14" s="1"/>
@@ -18791,20 +18975,20 @@
       <c r="L15" s="61"/>
       <c r="M15" s="70"/>
       <c r="N15"/>
-      <c r="O15" s="10">
+      <c r="O15" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P15" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R15" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S15" s="1"/>
@@ -18823,20 +19007,20 @@
       <c r="L16" s="33"/>
       <c r="M16" s="71"/>
       <c r="N16"/>
-      <c r="O16" s="10">
+      <c r="O16" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P16" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R16" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S16" s="1"/>
@@ -18856,20 +19040,20 @@
       <c r="L17" s="61"/>
       <c r="M17" s="58"/>
       <c r="N17"/>
-      <c r="O17" s="10">
+      <c r="O17" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P17" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S17" s="1"/>
@@ -18888,20 +19072,20 @@
       <c r="L18" s="33"/>
       <c r="M18" s="71"/>
       <c r="N18"/>
-      <c r="O18" s="10">
+      <c r="O18" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P18" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S18" s="1"/>
@@ -18921,20 +19105,20 @@
       <c r="L19" s="61"/>
       <c r="M19" s="58"/>
       <c r="N19"/>
-      <c r="O19" s="10">
+      <c r="O19" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P19" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q19" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R19" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S19" s="1"/>
@@ -18953,20 +19137,20 @@
       <c r="L20" s="33"/>
       <c r="M20" s="71"/>
       <c r="N20"/>
-      <c r="O20" s="10">
+      <c r="O20" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S20" s="1"/>
@@ -18986,20 +19170,20 @@
       <c r="L21" s="61"/>
       <c r="M21" s="70"/>
       <c r="N21"/>
-      <c r="O21" s="10">
+      <c r="O21" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P21" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q21" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R21" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S21" s="1"/>
@@ -19018,20 +19202,20 @@
       <c r="L22" s="33"/>
       <c r="M22" s="71"/>
       <c r="N22"/>
-      <c r="O22" s="10">
+      <c r="O22" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P22" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q22" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R22" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S22" s="1"/>
@@ -19051,20 +19235,20 @@
       <c r="L23" s="61"/>
       <c r="M23" s="70"/>
       <c r="N23"/>
-      <c r="O23" s="10">
+      <c r="O23" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P23" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q23" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R23" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S23" s="1"/>
@@ -19083,20 +19267,20 @@
       <c r="L24" s="33"/>
       <c r="M24" s="43"/>
       <c r="N24"/>
-      <c r="O24" s="10">
+      <c r="O24" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P24" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q24" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R24" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R24" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S24" s="1"/>
@@ -19116,20 +19300,20 @@
       <c r="L25" s="61"/>
       <c r="M25" s="70"/>
       <c r="N25"/>
-      <c r="O25" s="10">
+      <c r="O25" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P25" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q25" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R25" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R25" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S25" s="1"/>
@@ -19148,20 +19332,20 @@
       <c r="L26" s="33"/>
       <c r="M26" s="43"/>
       <c r="N26"/>
-      <c r="O26" s="10">
+      <c r="O26" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P26" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q26" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R26" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S26" s="1"/>
@@ -19181,20 +19365,20 @@
       <c r="L27" s="61"/>
       <c r="M27" s="70"/>
       <c r="N27"/>
-      <c r="O27" s="10">
+      <c r="O27" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P27" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q27" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R27" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R27" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S27" s="1"/>
@@ -19213,20 +19397,20 @@
       <c r="L28" s="33"/>
       <c r="M28" s="71"/>
       <c r="N28"/>
-      <c r="O28" s="10">
+      <c r="O28" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P28" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q28" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R28" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S28" s="1"/>
@@ -19246,20 +19430,20 @@
       <c r="L29" s="61"/>
       <c r="M29" s="70"/>
       <c r="N29"/>
-      <c r="O29" s="10">
+      <c r="O29" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P29" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q29" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R29" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S29" s="1"/>
@@ -19278,20 +19462,20 @@
       <c r="L30" s="33"/>
       <c r="M30" s="43"/>
       <c r="N30"/>
-      <c r="O30" s="10">
+      <c r="O30" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P30" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q30" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R30" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="10" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="S30" s="1"/>
@@ -19310,6 +19494,22 @@
       <c r="K31" s="57"/>
       <c r="L31" s="61"/>
       <c r="M31" s="70"/>
+      <c r="O31" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P31" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q31" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R31" s="10" t="str">
+        <f t="shared" ref="R31:R32" si="4">IF(OR(F31="",F31=0),"",(D31+F31)/10000)</f>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A32" s="31"/>
@@ -19325,6 +19525,22 @@
       <c r="K32" s="73"/>
       <c r="L32" s="71"/>
       <c r="M32" s="71"/>
+      <c r="O32" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P32" s="10" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="Q32" s="10" t="e">
+        <f t="shared" si="3"/>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" s="10" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
@@ -19341,12 +19557,22 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
-  <conditionalFormatting sqref="E3:E32">
+  <conditionalFormatting sqref="E32">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$E32&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32">
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>$L32&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E31">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$E3&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L32">
+  <conditionalFormatting sqref="L3:L31">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$L3&lt;0</formula>
     </cfRule>

</xml_diff>